<commit_message>
Update checks to get to 50% test coverage. And add in images to used add to vignettes
</commit_message>
<xml_diff>
--- a/tests/testthat/p21_mock.xlsx
+++ b/tests/testthat/p21_mock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cf124952\OneDrive - GSK\Documents\datadef\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{69B71B67-F127-41EB-81B5-40CD9B9DCA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{1923398E-2A38-4FD7-B6CC-69504DBB479B}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{69B71B67-F127-41EB-81B5-40CD9B9DCA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{C58A9013-E612-420D-A5B9-3057D25C7C47}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -2695,10 +2695,10 @@
   <dimension ref="A1:P258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D96" sqref="D96"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="37" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>49</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="38" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>49</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="80" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>51</v>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="81" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>51</v>

</xml_diff>